<commit_message>
new accepted and submitted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2627" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="1095">
   <si>
     <t>title</t>
   </si>
@@ -2940,12 +2940,6 @@
     <t>The health and economic burden of musculoskeletal disorders in Belgium from 2013 to 2018</t>
   </si>
   <si>
-    <t>Seminars in Arthritis &amp; Rheumatism</t>
-  </si>
-  <si>
-    <t>Semin. Arthritis Rheum.</t>
-  </si>
-  <si>
     <t>Gorasso, Vanessa; Van der Heyden, Johan; De Pauw, Robby; Pelgrims, Ingrid; De Clercq, Eva; De Ridder, Karin; Vandevijvere, Stefanie; Vansteelandt, Stijn; Vaes, Bert; De Smedt, Delphine; Devleesschauwer, Brecht</t>
   </si>
   <si>
@@ -3090,9 +3084,6 @@
     <t>Measuring small-area level deprivation in Belgium: the Belgian Index of Multiple Deprivation</t>
   </si>
   <si>
-    <t>Masquelier, Bruno; Faes, Christel; Van den Borre, Laura; Bouland, Catherine; De Clercq, Eva; Vandeninden, Bram; De Bleser, Andreas; Devleesschauwer, Brecht</t>
-  </si>
-  <si>
     <t>Spatial and Spatio-temporal Epidemiology</t>
   </si>
   <si>
@@ -3141,9 +3132,6 @@
     <t>Burden of disease attributable to risk factors in European countries: a systematic literature review</t>
   </si>
   <si>
-    <t>Gorasso,Vanessa; Nazaré Morgado, Joana; Charalampous, Periklis; Pires, Sara M.; Haagsma, Juanita A.; Santos, João Vasco: Idavain, Jane; Ngwa, Che Henry; Noguer, Isabel; Padron-Monedero, Alicia; Sarmiento, Rodrigo; Pinheiro, Vera; von der Lippe, Elena; Jakobsen, Lea Sletting; Devleesschauwer, Brecht; Plass, Dietrich; The COST Action CA18218 participants</t>
-  </si>
-  <si>
     <t>BMJ Global Health</t>
   </si>
   <si>
@@ -3295,6 +3283,33 @@
   </si>
   <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/36843241/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Challenges in Drug Surveillance: Strengthening the Analysis of New Psychoactive Substances by Harmonizing Drug Checking Services in Proficiency Testing </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/ijerph20054628</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/36901637/</t>
+  </si>
+  <si>
+    <t>Impact of environmental nitrogen pollution on pollen allergy: a scoping review</t>
+  </si>
+  <si>
+    <t>Sci. Total Environ.</t>
+  </si>
+  <si>
+    <t>Science of the Total Environment</t>
+  </si>
+  <si>
+    <t>Verscheure, Paulien; Honnay, Olivier; Speybroeck, Niko; Daelemans, Robin; Bruffaerts, Nicolas; Devleesschauwer, Brecht; Ceulemans, Tobias; Van Gerven, Laura; Aerts, Raf; Schrijvers, Rik</t>
+  </si>
+  <si>
+    <t>Otavova, Martina; Masquelier, Bruno; Faes, Christel; Van den Borre, Laura; Bouland, Catherine; De Clercq, Eva; Vandeninden, Bram; De Bleser, Andreas; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>Gorasso, Vanessa; Nazaré Morgado, Joana; Charalampous, Periklis; Pires, Sara M.; Haagsma, Juanita A.; Santos, João Vasco: Idavain, Jane; Ngwa, Che Henry; Noguer, Isabel; Padron-Monedero, Alicia; Sarmiento, Rodrigo; Pinheiro, Vera; von der Lippe, Elena; Jakobsen, Lea Sletting; Devleesschauwer, Brecht; Plass, Dietrich; The COST Action CA18218 participants</t>
   </si>
 </sst>
 </file>
@@ -3411,7 +3426,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3548,9 +3563,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3603,169 +3615,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4007,6 +3856,169 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -4021,74 +4033,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U218" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:U218"/>
-  <sortState ref="A2:U218">
-    <sortCondition ref="K1:K218"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U221" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+  <autoFilter ref="A1:U221"/>
+  <sortState ref="A2:U221">
+    <sortCondition ref="K1:K221"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="51"/>
-    <tableColumn id="2" name="authors" dataDxfId="50"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="49"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="48"/>
-    <tableColumn id="6" name="year" dataDxfId="47"/>
-    <tableColumn id="4" name="volume" dataDxfId="46"/>
-    <tableColumn id="5" name="issue" dataDxfId="45"/>
-    <tableColumn id="7" name="eID" dataDxfId="44"/>
-    <tableColumn id="8" name="from" dataDxfId="43"/>
-    <tableColumn id="9" name="to" dataDxfId="42"/>
-    <tableColumn id="10" name="date" dataDxfId="41"/>
-    <tableColumn id="14" name="classification" dataDxfId="40"/>
-    <tableColumn id="12" name="IF" dataDxfId="39"/>
-    <tableColumn id="13" name="DOI" dataDxfId="38"/>
-    <tableColumn id="15" name="WoS" dataDxfId="37"/>
-    <tableColumn id="16" name="rank" dataDxfId="36"/>
-    <tableColumn id="17" name="quartile" dataDxfId="35"/>
-    <tableColumn id="18" name="category" dataDxfId="34"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="33"/>
-    <tableColumn id="20" name="SC" dataDxfId="32"/>
-    <tableColumn id="21" name="UGent" dataDxfId="31"/>
+    <tableColumn id="1" name="title" dataDxfId="75"/>
+    <tableColumn id="2" name="authors" dataDxfId="74"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="73"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="72"/>
+    <tableColumn id="6" name="year" dataDxfId="71"/>
+    <tableColumn id="4" name="volume" dataDxfId="70"/>
+    <tableColumn id="5" name="issue" dataDxfId="69"/>
+    <tableColumn id="7" name="eID" dataDxfId="68"/>
+    <tableColumn id="8" name="from" dataDxfId="67"/>
+    <tableColumn id="9" name="to" dataDxfId="66"/>
+    <tableColumn id="10" name="date" dataDxfId="65"/>
+    <tableColumn id="14" name="classification" dataDxfId="64"/>
+    <tableColumn id="12" name="IF" dataDxfId="63"/>
+    <tableColumn id="13" name="DOI" dataDxfId="62"/>
+    <tableColumn id="15" name="WoS" dataDxfId="61"/>
+    <tableColumn id="16" name="rank" dataDxfId="60"/>
+    <tableColumn id="17" name="quartile" dataDxfId="59"/>
+    <tableColumn id="18" name="category" dataDxfId="58"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="57"/>
+    <tableColumn id="20" name="SC" dataDxfId="56"/>
+    <tableColumn id="21" name="UGent" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J11" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J11" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="A1:J11"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="29"/>
-    <tableColumn id="2" name="authors" dataDxfId="28"/>
-    <tableColumn id="3" name="editors" dataDxfId="27"/>
-    <tableColumn id="11" name="book" dataDxfId="26"/>
-    <tableColumn id="6" name="year" dataDxfId="25"/>
-    <tableColumn id="8" name="from" dataDxfId="24"/>
-    <tableColumn id="9" name="to" dataDxfId="23"/>
-    <tableColumn id="10" name="date" dataDxfId="22"/>
-    <tableColumn id="12" name="IF" dataDxfId="21"/>
-    <tableColumn id="13" name="DOI" dataDxfId="20"/>
+    <tableColumn id="1" name="title" dataDxfId="53"/>
+    <tableColumn id="2" name="authors" dataDxfId="52"/>
+    <tableColumn id="3" name="editors" dataDxfId="51"/>
+    <tableColumn id="11" name="book" dataDxfId="50"/>
+    <tableColumn id="6" name="year" dataDxfId="49"/>
+    <tableColumn id="8" name="from" dataDxfId="48"/>
+    <tableColumn id="9" name="to" dataDxfId="47"/>
+    <tableColumn id="10" name="date" dataDxfId="46"/>
+    <tableColumn id="12" name="IF" dataDxfId="45"/>
+    <tableColumn id="13" name="DOI" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:G18" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:G18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:G16" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:G16"/>
   <sortState ref="A2:G17">
     <sortCondition ref="F1:F17"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="title" dataDxfId="17"/>
-    <tableColumn id="2" name="authors" dataDxfId="16"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="15"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="14"/>
-    <tableColumn id="4" name="doi_preprint" dataDxfId="13"/>
-    <tableColumn id="10" name="date" dataDxfId="12"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="11">
+    <tableColumn id="1" name="title" dataDxfId="41"/>
+    <tableColumn id="2" name="authors" dataDxfId="40"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="39"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="38"/>
+    <tableColumn id="4" name="doi_preprint" dataDxfId="37"/>
+    <tableColumn id="10" name="date" dataDxfId="36"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="35">
       <calculatedColumnFormula>TODAY()-F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4097,18 +4109,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="8"/>
-    <tableColumn id="2" name="authors" dataDxfId="7"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="6"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="5"/>
-    <tableColumn id="10" name="date" dataDxfId="4"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="3">
+    <tableColumn id="1" name="title" dataDxfId="32"/>
+    <tableColumn id="2" name="authors" dataDxfId="31"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="30"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="29"/>
+    <tableColumn id="10" name="date" dataDxfId="28"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="27">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4403,10 +4415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U218"/>
+  <dimension ref="A1:U221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView topLeftCell="A188" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14257,10 +14269,10 @@
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="C180" s="7" t="s">
         <v>575</v>
@@ -14294,7 +14306,7 @@
       </c>
       <c r="M180" s="11"/>
       <c r="N180" s="19" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="O180" s="7"/>
       <c r="P180" s="24"/>
@@ -15195,7 +15207,7 @@
       </c>
       <c r="M197" s="11"/>
       <c r="N197" s="19" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="O197" s="7"/>
       <c r="P197" s="24"/>
@@ -15211,16 +15223,16 @@
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>980</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="D198" s="7" t="s">
         <v>978</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>982</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>979</v>
-      </c>
-      <c r="D198" s="7" t="s">
-        <v>980</v>
       </c>
       <c r="E198" s="18">
         <v>2022</v>
@@ -15248,7 +15260,7 @@
       </c>
       <c r="M198" s="11"/>
       <c r="N198" s="19" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="O198" s="7"/>
       <c r="P198" s="24"/>
@@ -15301,7 +15313,7 @@
       </c>
       <c r="M199" s="11"/>
       <c r="N199" s="19" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="O199" s="7"/>
       <c r="P199" s="24"/>
@@ -15354,7 +15366,7 @@
       </c>
       <c r="M200" s="11"/>
       <c r="N200" s="19" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="O200" s="7"/>
       <c r="P200" s="24"/>
@@ -15407,7 +15419,7 @@
       </c>
       <c r="M201" s="11"/>
       <c r="N201" s="19" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="O201" s="7"/>
       <c r="P201" s="24"/>
@@ -15460,7 +15472,7 @@
       </c>
       <c r="M202" s="11"/>
       <c r="N202" s="19" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="O202" s="7"/>
       <c r="P202" s="24"/>
@@ -15482,10 +15494,10 @@
         <v>969</v>
       </c>
       <c r="C203" s="7" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D203" s="7" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E203" s="18">
         <v>2022</v>
@@ -15513,7 +15525,7 @@
       </c>
       <c r="M203" s="11"/>
       <c r="N203" s="19" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="O203" s="7"/>
       <c r="P203" s="24"/>
@@ -15566,7 +15578,7 @@
       </c>
       <c r="M204" s="11"/>
       <c r="N204" s="19" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="O204" s="7"/>
       <c r="P204" s="24"/>
@@ -15582,7 +15594,7 @@
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B205" s="7" t="s">
         <v>935</v>
@@ -15603,7 +15615,7 @@
         <v>69</v>
       </c>
       <c r="H205" s="18" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="I205" s="18" t="s">
         <v>14</v>
@@ -15619,7 +15631,7 @@
       </c>
       <c r="M205" s="11"/>
       <c r="N205" s="19" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="O205" s="7"/>
       <c r="P205" s="24"/>
@@ -15672,7 +15684,7 @@
       </c>
       <c r="M206" s="11"/>
       <c r="N206" s="19" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="O206" s="7"/>
       <c r="P206" s="24"/>
@@ -15725,7 +15737,7 @@
       </c>
       <c r="M207" s="11"/>
       <c r="N207" s="19" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="O207" s="7"/>
       <c r="P207" s="24"/>
@@ -15815,7 +15827,7 @@
         <v>65</v>
       </c>
       <c r="H209" s="18" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="I209" s="18" t="s">
         <v>14</v>
@@ -15831,7 +15843,7 @@
       </c>
       <c r="M209" s="11"/>
       <c r="N209" s="19" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="O209" s="7"/>
       <c r="P209" s="24"/>
@@ -15884,7 +15896,7 @@
       </c>
       <c r="M210" s="11"/>
       <c r="N210" s="19" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="O210" s="7"/>
       <c r="P210" s="24"/>
@@ -15900,28 +15912,28 @@
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
-        <v>1009</v>
+        <v>995</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>1073</v>
+        <v>996</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>509</v>
+        <v>997</v>
       </c>
       <c r="D211" s="7" t="s">
-        <v>510</v>
+        <v>998</v>
       </c>
       <c r="E211" s="18">
         <v>2023</v>
       </c>
       <c r="F211" s="18">
-        <v>151</v>
+        <v>30</v>
       </c>
       <c r="G211" s="19" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="H211" s="18" t="s">
-        <v>1085</v>
+        <v>999</v>
       </c>
       <c r="I211" s="18" t="s">
         <v>14</v>
@@ -15930,14 +15942,14 @@
         <v>14</v>
       </c>
       <c r="K211" s="42">
-        <v>44935</v>
+        <v>44927</v>
       </c>
       <c r="L211" s="42" t="s">
         <v>273</v>
       </c>
       <c r="M211" s="11"/>
       <c r="N211" s="19" t="s">
-        <v>1078</v>
+        <v>1000</v>
       </c>
       <c r="O211" s="7"/>
       <c r="P211" s="24"/>
@@ -15953,28 +15965,28 @@
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
-        <v>940</v>
+        <v>1007</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>941</v>
+        <v>1069</v>
       </c>
       <c r="C212" s="7" t="s">
-        <v>144</v>
+        <v>509</v>
       </c>
       <c r="D212" s="7" t="s">
-        <v>144</v>
+        <v>510</v>
       </c>
       <c r="E212" s="18">
         <v>2023</v>
       </c>
       <c r="F212" s="18">
-        <v>18</v>
+        <v>151</v>
       </c>
       <c r="G212" s="19" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="H212" s="18" t="s">
-        <v>1075</v>
+        <v>1081</v>
       </c>
       <c r="I212" s="18" t="s">
         <v>14</v>
@@ -15983,14 +15995,14 @@
         <v>14</v>
       </c>
       <c r="K212" s="42">
-        <v>44950</v>
+        <v>44935</v>
       </c>
       <c r="L212" s="42" t="s">
         <v>273</v>
       </c>
       <c r="M212" s="11"/>
       <c r="N212" s="19" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="O212" s="7"/>
       <c r="P212" s="24"/>
@@ -16006,28 +16018,28 @@
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>1065</v>
+        <v>940</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>926</v>
+        <v>941</v>
       </c>
       <c r="C213" s="7" t="s">
-        <v>1066</v>
+        <v>144</v>
       </c>
       <c r="D213" s="7" t="s">
-        <v>1067</v>
+        <v>144</v>
       </c>
       <c r="E213" s="18">
         <v>2023</v>
       </c>
       <c r="F213" s="18">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G213" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H213" s="18">
-        <v>1063982</v>
+        <v>101</v>
+      </c>
+      <c r="H213" s="18" t="s">
+        <v>1071</v>
       </c>
       <c r="I213" s="18" t="s">
         <v>14</v>
@@ -16036,14 +16048,14 @@
         <v>14</v>
       </c>
       <c r="K213" s="42">
-        <v>44959</v>
+        <v>44950</v>
       </c>
       <c r="L213" s="42" t="s">
         <v>273</v>
       </c>
       <c r="M213" s="11"/>
       <c r="N213" s="19" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
       <c r="O213" s="7"/>
       <c r="P213" s="24"/>
@@ -16059,44 +16071,44 @@
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
-        <v>1086</v>
+        <v>1061</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>974</v>
+        <v>926</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>287</v>
+        <v>1062</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>330</v>
+        <v>1063</v>
       </c>
       <c r="E214" s="18">
         <v>2023</v>
       </c>
       <c r="F214" s="18">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="G214" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H214" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I214" s="18">
-        <v>121</v>
-      </c>
-      <c r="J214" s="18">
-        <v>126</v>
+        <v>14</v>
+      </c>
+      <c r="H214" s="18">
+        <v>1063982</v>
+      </c>
+      <c r="I214" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J214" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="K214" s="42">
-        <v>44960</v>
+        <v>44959</v>
       </c>
       <c r="L214" s="42" t="s">
         <v>273</v>
       </c>
       <c r="M214" s="11"/>
       <c r="N214" s="19" t="s">
-        <v>1011</v>
+        <v>1073</v>
       </c>
       <c r="O214" s="7"/>
       <c r="P214" s="24"/>
@@ -16112,22 +16124,22 @@
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>791</v>
+        <v>1082</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>792</v>
+        <v>972</v>
       </c>
       <c r="C215" s="7" t="s">
-        <v>790</v>
+        <v>287</v>
       </c>
       <c r="D215" s="7" t="s">
-        <v>793</v>
+        <v>330</v>
       </c>
       <c r="E215" s="18">
         <v>2023</v>
       </c>
       <c r="F215" s="18">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="G215" s="19" t="s">
         <v>101</v>
@@ -16136,20 +16148,20 @@
         <v>14</v>
       </c>
       <c r="I215" s="18">
-        <v>296</v>
+        <v>121</v>
       </c>
       <c r="J215" s="18">
-        <v>300</v>
+        <v>126</v>
       </c>
       <c r="K215" s="42">
-        <v>44986</v>
+        <v>44960</v>
       </c>
       <c r="L215" s="42" t="s">
         <v>273</v>
       </c>
       <c r="M215" s="11"/>
       <c r="N215" s="19" t="s">
-        <v>827</v>
+        <v>1009</v>
       </c>
       <c r="O215" s="7"/>
       <c r="P215" s="24"/>
@@ -16164,66 +16176,70 @@
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A216" s="13" t="s">
-        <v>989</v>
-      </c>
-      <c r="B216" s="13" t="s">
-        <v>990</v>
-      </c>
-      <c r="C216" s="13" t="s">
-        <v>991</v>
-      </c>
-      <c r="D216" s="13" t="s">
-        <v>992</v>
-      </c>
-      <c r="E216" s="14">
+      <c r="A216" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="C216" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="D216" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="E216" s="18">
         <v>2023</v>
       </c>
-      <c r="F216" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G216" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H216" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I216" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J216" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K216" s="31">
-        <v>45293</v>
-      </c>
-      <c r="L216" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="M216" s="45"/>
-      <c r="N216" s="44" t="s">
-        <v>996</v>
-      </c>
-      <c r="O216" s="27"/>
+      <c r="F216" s="18">
+        <v>5</v>
+      </c>
+      <c r="G216" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H216" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I216" s="18">
+        <v>296</v>
+      </c>
+      <c r="J216" s="18">
+        <v>300</v>
+      </c>
+      <c r="K216" s="42">
+        <v>44986</v>
+      </c>
+      <c r="L216" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="M216" s="11"/>
+      <c r="N216" s="19" t="s">
+        <v>827</v>
+      </c>
+      <c r="O216" s="7"/>
       <c r="P216" s="24"/>
       <c r="Q216" s="25"/>
       <c r="R216" s="7"/>
       <c r="S216" s="7"/>
-      <c r="T216" s="7"/>
-      <c r="U216" s="7"/>
+      <c r="T216" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="U216" s="7" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="13" t="s">
-        <v>997</v>
+        <v>987</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>998</v>
+        <v>988</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>999</v>
+        <v>989</v>
       </c>
       <c r="D217" s="13" t="s">
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="E217" s="14">
         <v>2023</v>
@@ -16235,7 +16251,7 @@
         <v>14</v>
       </c>
       <c r="H217" s="43" t="s">
-        <v>1001</v>
+        <v>14</v>
       </c>
       <c r="I217" s="43" t="s">
         <v>14</v>
@@ -16244,14 +16260,14 @@
         <v>14</v>
       </c>
       <c r="K217" s="31">
-        <v>45294</v>
-      </c>
-      <c r="L217" s="48" t="s">
+        <v>45292</v>
+      </c>
+      <c r="L217" s="31" t="s">
         <v>273</v>
       </c>
       <c r="M217" s="45"/>
       <c r="N217" s="44" t="s">
-        <v>1002</v>
+        <v>994</v>
       </c>
       <c r="O217" s="27"/>
       <c r="P217" s="24"/>
@@ -16263,16 +16279,16 @@
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="13" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B218" s="13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C218" s="13" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D218" s="13" t="s">
         <v>1033</v>
-      </c>
-      <c r="B218" s="13" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C218" s="13" t="s">
-        <v>1034</v>
-      </c>
-      <c r="D218" s="13" t="s">
-        <v>1036</v>
       </c>
       <c r="E218" s="14">
         <v>2023</v>
@@ -16293,14 +16309,14 @@
         <v>14</v>
       </c>
       <c r="K218" s="31">
-        <v>45297</v>
+        <v>45293</v>
       </c>
       <c r="L218" s="31" t="s">
         <v>273</v>
       </c>
       <c r="M218" s="45"/>
       <c r="N218" s="44" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="O218" s="27"/>
       <c r="P218" s="24"/>
@@ -16310,100 +16326,241 @@
       <c r="T218" s="7"/>
       <c r="U218" s="7"/>
     </row>
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A219" s="13" t="s">
+        <v>931</v>
+      </c>
+      <c r="B219" s="13" t="s">
+        <v>767</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>932</v>
+      </c>
+      <c r="D219" s="13" t="s">
+        <v>933</v>
+      </c>
+      <c r="E219" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F219" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G219" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H219" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I219" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J219" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K219" s="31">
+        <v>45294</v>
+      </c>
+      <c r="L219" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="M219" s="45"/>
+      <c r="N219" s="44"/>
+      <c r="O219" s="27"/>
+      <c r="P219" s="24"/>
+      <c r="Q219" s="25"/>
+      <c r="R219" s="7"/>
+      <c r="S219" s="7"/>
+      <c r="T219" s="7"/>
+      <c r="U219" s="7"/>
+    </row>
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A220" s="13" t="s">
+        <v>970</v>
+      </c>
+      <c r="B220" s="13" t="s">
+        <v>971</v>
+      </c>
+      <c r="C220" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D220" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E220" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F220" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G220" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H220" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I220" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J220" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K220" s="31">
+        <v>45295</v>
+      </c>
+      <c r="L220" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="M220" s="45"/>
+      <c r="N220" s="44"/>
+      <c r="O220" s="27"/>
+      <c r="P220" s="24"/>
+      <c r="Q220" s="25"/>
+      <c r="R220" s="7"/>
+      <c r="S220" s="7"/>
+      <c r="T220" s="7"/>
+      <c r="U220" s="7"/>
+    </row>
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A221" s="13" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B221" s="13" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C221" s="13" t="s">
+        <v>724</v>
+      </c>
+      <c r="D221" s="13" t="s">
+        <v>724</v>
+      </c>
+      <c r="E221" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F221" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G221" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H221" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I221" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J221" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K221" s="31">
+        <v>45296</v>
+      </c>
+      <c r="L221" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="M221" s="45"/>
+      <c r="N221" s="44"/>
+      <c r="O221" s="27"/>
+      <c r="P221" s="24"/>
+      <c r="Q221" s="25"/>
+      <c r="R221" s="7"/>
+      <c r="S221" s="7"/>
+      <c r="T221" s="7"/>
+      <c r="U221" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S148:U175 S136:U146 S177:U179 S182:U188 S190:U205 S207:U1048576">
-    <cfRule type="cellIs" dxfId="77" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="75" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="73" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="71" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="67" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S147:U147">
-    <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S176:U176">
-    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S181:U181">
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S189:U189">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S206:U206">
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S180:U180">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16775,11 +16932,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16815,378 +16970,334 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>931</v>
+        <v>960</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>767</v>
+        <v>961</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>932</v>
+        <v>959</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>933</v>
+        <v>962</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="10">
-        <v>44191</v>
+        <v>44734</v>
       </c>
       <c r="G2" s="12">
-        <f t="shared" ref="G2:G18" ca="1" si="0">TODAY()-F2</f>
-        <v>799</v>
+        <f t="shared" ref="G2:G16" ca="1" si="0">TODAY()-F2</f>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>960</v>
+        <v>973</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>961</v>
+        <v>974</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>959</v>
+        <v>89</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>962</v>
-      </c>
-      <c r="E3" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1078</v>
+      </c>
       <c r="F3" s="10">
-        <v>44734</v>
+        <v>44769</v>
       </c>
       <c r="G3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>970</v>
+        <v>991</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>973</v>
+        <v>992</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>971</v>
+        <v>659</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>972</v>
+        <v>660</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="10">
-        <v>44757</v>
+        <v>44803</v>
       </c>
       <c r="G4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>233</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>975</v>
+        <v>983</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>976</v>
+        <v>984</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>89</v>
+        <v>669</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>1082</v>
-      </c>
+        <v>670</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="10">
-        <v>44769</v>
+        <v>44810</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>221</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>993</v>
+        <v>981</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>994</v>
+        <v>982</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>659</v>
+        <v>790</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>660</v>
+        <v>793</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="10">
-        <v>44803</v>
+        <v>44832</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>985</v>
+        <v>1013</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>986</v>
+        <v>1014</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>669</v>
+        <v>144</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>670</v>
+        <v>144</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="10">
-        <v>44810</v>
+        <v>44883</v>
       </c>
       <c r="G7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>983</v>
+        <v>1018</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>984</v>
+        <v>1093</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>790</v>
+        <v>1019</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>793</v>
+        <v>1020</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="10">
-        <v>44832</v>
+        <v>44897</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>1004</v>
+        <v>1016</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1005</v>
+        <v>1017</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>724</v>
+        <v>1021</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>724</v>
+        <v>1022</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="10">
-        <v>44852</v>
+        <v>44902</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>138</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>1015</v>
+        <v>1024</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1016</v>
+        <v>1023</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>144</v>
+        <v>1025</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="10">
-        <v>44883</v>
+        <v>44904</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>1020</v>
+        <v>1034</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1021</v>
+        <v>1094</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1022</v>
+        <v>1035</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>1023</v>
+        <v>1036</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="10">
-        <v>44897</v>
+        <v>44914</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>1018</v>
+        <v>1037</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1019</v>
+        <v>1038</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1024</v>
+        <v>1035</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>1025</v>
+        <v>1036</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="10">
-        <v>44902</v>
+        <v>44914</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>1027</v>
+        <v>1064</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1026</v>
+        <v>1065</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1028</v>
+        <v>259</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>82</v>
+        <v>262</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="10">
-        <v>44904</v>
+        <v>44942</v>
       </c>
       <c r="G13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>1037</v>
+        <v>1076</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1038</v>
+        <v>1077</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>1039</v>
+        <v>25</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>1040</v>
+        <v>28</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="10">
-        <v>44914</v>
+        <v>44958</v>
       </c>
       <c r="G14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>1041</v>
+        <v>1079</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>1042</v>
+        <v>1080</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1039</v>
+        <v>120</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>1040</v>
+        <v>121</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="10">
-        <v>44914</v>
+        <v>44959</v>
       </c>
       <c r="G15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>1068</v>
+        <v>1089</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>1069</v>
+        <v>1092</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>259</v>
+        <v>1091</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>262</v>
+        <v>1090</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="10">
-        <v>44942</v>
+        <v>45008</v>
       </c>
       <c r="G16" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="10">
-        <v>44958</v>
-      </c>
-      <c r="G17" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>1083</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>1084</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="10">
-        <v>44959</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -17251,7 +17362,7 @@
       </c>
       <c r="F2" s="40">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>7.3479452054794523</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -17272,7 +17383,7 @@
       </c>
       <c r="F3" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3479452054794523</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -17293,7 +17404,7 @@
       </c>
       <c r="F4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7260273972602738</v>
+        <v>6.7780821917808218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -17314,7 +17425,7 @@
       </c>
       <c r="F5" s="40">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>5.095890410958904</v>
+        <v>5.1479452054794521</v>
       </c>
     </row>
   </sheetData>
@@ -17327,158 +17438,173 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="81.28515625" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="15"/>
-    <col min="5" max="9" width="9.140625" style="49"/>
+    <col min="5" max="9" width="9.140625" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="51">
+      <c r="E1" s="50">
         <f>COUNTA(E3:E998)</f>
         <v>2</v>
       </c>
-      <c r="F1" s="51">
+      <c r="F1" s="50">
         <f>COUNTA(F3:F998)</f>
         <v>0</v>
       </c>
-      <c r="G1" s="51">
+      <c r="G1" s="50">
         <f>COUNTA(G3:G998)</f>
-        <v>0</v>
-      </c>
-      <c r="H1" s="51">
+        <v>1</v>
+      </c>
+      <c r="H1" s="50">
         <f>COUNTA(H3:H998)</f>
         <v>2</v>
       </c>
-      <c r="I1" s="51">
+      <c r="I1" s="50">
         <f>COUNTA(I3:I998)</f>
         <v>1</v>
       </c>
-      <c r="J1" s="52">
+      <c r="J1" s="51">
         <f>SUM(E1:I1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>1062</v>
-      </c>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="52" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="53" t="s">
-        <v>1063</v>
-      </c>
-      <c r="D2" s="53" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E2" s="54" t="s">
-        <v>1048</v>
-      </c>
-      <c r="F2" s="54" t="s">
+      <c r="C2" s="52" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H2" s="53" t="s">
+        <v>1046</v>
+      </c>
+      <c r="I2" s="53" t="s">
         <v>1047</v>
-      </c>
-      <c r="G2" s="54" t="s">
-        <v>1049</v>
-      </c>
-      <c r="H2" s="54" t="s">
-        <v>1050</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>1053</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>1054</v>
+        <v>1042</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>1050</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1061</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>1052</v>
+        <v>1057</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>1056</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>1057</v>
+        <v>1051</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>1053</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>1074</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>1052</v>
+        <v>1070</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>1060</v>
+        <v>1054</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>1056</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E5" s="49" t="s">
-        <v>1052</v>
+        <v>1070</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>1072</v>
+        <v>1066</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>1068</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>1061</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>1052</v>
+        <v>1057</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>1087</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="C8" s="49" t="s">
         <v>1088</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>1061</v>
-      </c>
-      <c r="H7" s="49" t="s">
-        <v>1052</v>
+      <c r="D8" s="15" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>1048</v>
       </c>
     </row>
   </sheetData>
@@ -17506,8 +17632,10 @@
     <hyperlink ref="C6" r:id="rId8"/>
     <hyperlink ref="B7" r:id="rId9"/>
     <hyperlink ref="C7" r:id="rId10"/>
+    <hyperlink ref="B8" r:id="rId11"/>
+    <hyperlink ref="C8" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new submissions and accepted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="1162">
   <si>
     <t>title</t>
   </si>
@@ -3138,9 +3138,6 @@
     <t>e0010468</t>
   </si>
   <si>
-    <t xml:space="preserve"> Self-uniqueness beliefs and adherence to recommended precautions. A 5-wave longitudinal COVID-19 study </t>
-  </si>
-  <si>
     <t>HIND</t>
   </si>
   <si>
@@ -3165,18 +3162,12 @@
     <t>https://pubmed.ncbi.nlm.nih.gov/36495770/</t>
   </si>
   <si>
-    <t xml:space="preserve"> Innovative Methods Used in Monitoring COVID-19 in Europe: A Multinational Study </t>
-  </si>
-  <si>
     <t>https://doi.org/10.3390/ijerph20010564</t>
   </si>
   <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/36612884/</t>
   </si>
   <si>
-    <t xml:space="preserve"> Prevalence and factors associated with academic burnout risk among nursing and midwifery students during the COVID-19 pandemic: A cross-sectional study </t>
-  </si>
-  <si>
     <t>https://doi.org/10.1002/nop2.1575</t>
   </si>
   <si>
@@ -3210,9 +3201,6 @@
     <t>Nayani, Sarah; Castañares, Diego; De Pauw, Robby; Van Cauteren, Dieter; Demarest, Stefaan; Drieskens, Sabine; Cornelissen, Laura; Devleesschauwer, Brecht; De Ridder, Karin; Charafeddine, Rana; Smith, Pierre</t>
   </si>
   <si>
-    <t xml:space="preserve"> National Trends and Disparities in Retail Food Environments in the United States between 1990-2014</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1017/s1368980023000058</t>
   </si>
   <si>
@@ -3261,9 +3249,6 @@
     <t>Burden of disease among older adults in Europe-trends in mortality and disability, 1990-2019</t>
   </si>
   <si>
-    <t xml:space="preserve"> Product promotional strategies in supermarkets and their effects on sales: A case study of breakfast cereals and drinks in New Zealand </t>
-  </si>
-  <si>
     <t>https://doi.org/10.1111/1747-0080.12800</t>
   </si>
   <si>
@@ -3459,13 +3444,73 @@
     <t>10.3389/ijph.2023.1605763</t>
   </si>
   <si>
-    <t>rs-2952989/v1</t>
-  </si>
-  <si>
     <t>Investigating years of life lost in Belgium, 2004–2019: A comprehensive analysis using a probabilistic redistribution approach</t>
   </si>
   <si>
     <t>Devleesschauwer, Brecht; Scohy, Aline; De Pauw, Robby; Gorasso, Vanessa; Kongs, Anne; Neirynck, Elias; Verduyckt, Peter; Wyper, Grant M A; Van den Borre, Laura</t>
+  </si>
+  <si>
+    <t>10.21203/rs.3.rs-2952989/v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trends in adults' energy imbalance gaps over two decades in Belgium using system dynamics modelling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product promotional strategies in supermarkets and their effects on sales: A case study of breakfast cereals and drinks in New Zealand </t>
+  </si>
+  <si>
+    <t>National Trends and Disparities in Retail Food Environments in the United States between 1990-2014</t>
+  </si>
+  <si>
+    <t>Prevalence and factors associated with academic burnout risk among nursing and midwifery students during the COVID-19 pandemic: A cross-sectional study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Innovative Methods Used in Monitoring COVID-19 in Europe: A Multinational Study </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-uniqueness beliefs and adherence to recommended precautions. A 5-wave longitudinal COVID-19 study </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s40795-023-00721-0</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37245052/</t>
+  </si>
+  <si>
+    <t>Assessing European national health information systems in peer review format: lessons learnt</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/eurpub/ckad085</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37263589/</t>
+  </si>
+  <si>
+    <t>Di Bari, Carlotta; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>Burden of Foodborne Diseases From Biological Hazards</t>
+  </si>
+  <si>
+    <t>10.1016/B978-0-12-822521-9.00221-5</t>
+  </si>
+  <si>
+    <t>The state of health in the European Union (EU-27) in 2019: A systematic analysis for the Global Burden of Disease Study 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMC Public Health </t>
+  </si>
+  <si>
+    <t>Gorasso, Vanessa; Vandevijvere, Stefanie; Heyden, Johan Van der; Pelgrims, Ingrid; Hilderink, Henk; Nusselder, Wilma; Demoury, Claire; Schmidt, Masja; Vansteelandt, Stijn; Smedt, Delphine De; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>Cancer Medicine</t>
+  </si>
+  <si>
+    <t>Cancer Med.</t>
+  </si>
+  <si>
+    <t>Santos, João Vasco, Devleesschauwer, Brecht</t>
   </si>
 </sst>
 </file>
@@ -3741,7 +3786,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="80">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3771,169 +3816,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4175,6 +4057,189 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -4189,74 +4254,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U224" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:U224"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U226" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+  <autoFilter ref="A1:U226"/>
   <sortState ref="A2:U224">
     <sortCondition ref="K1:K224"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="51"/>
-    <tableColumn id="2" name="authors" dataDxfId="50"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="49"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="48"/>
-    <tableColumn id="6" name="year" dataDxfId="47"/>
-    <tableColumn id="4" name="volume" dataDxfId="46"/>
-    <tableColumn id="5" name="issue" dataDxfId="45"/>
-    <tableColumn id="7" name="eID" dataDxfId="44"/>
-    <tableColumn id="8" name="from" dataDxfId="43"/>
-    <tableColumn id="9" name="to" dataDxfId="42"/>
-    <tableColumn id="10" name="date" dataDxfId="41"/>
-    <tableColumn id="14" name="classification" dataDxfId="40"/>
-    <tableColumn id="12" name="IF" dataDxfId="39"/>
-    <tableColumn id="13" name="DOI" dataDxfId="38"/>
-    <tableColumn id="15" name="WoS" dataDxfId="37"/>
-    <tableColumn id="16" name="rank" dataDxfId="36"/>
-    <tableColumn id="17" name="quartile" dataDxfId="35"/>
-    <tableColumn id="18" name="category" dataDxfId="34"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="33"/>
-    <tableColumn id="20" name="SC" dataDxfId="32"/>
-    <tableColumn id="21" name="UGent" dataDxfId="31"/>
+    <tableColumn id="1" name="title" dataDxfId="77"/>
+    <tableColumn id="2" name="authors" dataDxfId="76"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="75"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="74"/>
+    <tableColumn id="6" name="year" dataDxfId="73"/>
+    <tableColumn id="4" name="volume" dataDxfId="72"/>
+    <tableColumn id="5" name="issue" dataDxfId="71"/>
+    <tableColumn id="7" name="eID" dataDxfId="70"/>
+    <tableColumn id="8" name="from" dataDxfId="69"/>
+    <tableColumn id="9" name="to" dataDxfId="68"/>
+    <tableColumn id="10" name="date" dataDxfId="67"/>
+    <tableColumn id="14" name="classification" dataDxfId="66"/>
+    <tableColumn id="12" name="IF" dataDxfId="65"/>
+    <tableColumn id="13" name="DOI" dataDxfId="64"/>
+    <tableColumn id="15" name="WoS" dataDxfId="63"/>
+    <tableColumn id="16" name="rank" dataDxfId="62"/>
+    <tableColumn id="17" name="quartile" dataDxfId="61"/>
+    <tableColumn id="18" name="category" dataDxfId="60"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="59"/>
+    <tableColumn id="20" name="SC" dataDxfId="58"/>
+    <tableColumn id="21" name="UGent" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J11" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A1:J11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J12" totalsRowShown="0" headerRowDxfId="56">
+  <autoFilter ref="A1:J12"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="29"/>
-    <tableColumn id="2" name="authors" dataDxfId="28"/>
-    <tableColumn id="3" name="editors" dataDxfId="27"/>
-    <tableColumn id="11" name="book" dataDxfId="26"/>
-    <tableColumn id="6" name="year" dataDxfId="25"/>
-    <tableColumn id="8" name="from" dataDxfId="24"/>
-    <tableColumn id="9" name="to" dataDxfId="23"/>
-    <tableColumn id="10" name="date" dataDxfId="22"/>
-    <tableColumn id="12" name="IF" dataDxfId="21"/>
-    <tableColumn id="13" name="DOI" dataDxfId="20"/>
+    <tableColumn id="1" name="title" dataDxfId="55"/>
+    <tableColumn id="2" name="authors" dataDxfId="54"/>
+    <tableColumn id="3" name="editors" dataDxfId="53"/>
+    <tableColumn id="11" name="book" dataDxfId="52"/>
+    <tableColumn id="6" name="year" dataDxfId="51"/>
+    <tableColumn id="8" name="from" dataDxfId="50"/>
+    <tableColumn id="9" name="to" dataDxfId="49"/>
+    <tableColumn id="10" name="date" dataDxfId="48"/>
+    <tableColumn id="12" name="IF" dataDxfId="47"/>
+    <tableColumn id="13" name="DOI" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:G24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:G24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:G23" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="A1:G23"/>
   <sortState ref="A2:G17">
     <sortCondition ref="F1:F17"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="title" dataDxfId="17"/>
-    <tableColumn id="2" name="authors" dataDxfId="16"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="15"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="14"/>
-    <tableColumn id="4" name="doi_preprint" dataDxfId="13"/>
-    <tableColumn id="10" name="date" dataDxfId="12"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="11">
+    <tableColumn id="1" name="title" dataDxfId="43"/>
+    <tableColumn id="2" name="authors" dataDxfId="42"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="41"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="40"/>
+    <tableColumn id="4" name="doi_preprint" dataDxfId="39"/>
+    <tableColumn id="10" name="date" dataDxfId="38"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="37">
       <calculatedColumnFormula>TODAY()-F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4265,18 +4330,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="8"/>
-    <tableColumn id="2" name="authors" dataDxfId="7"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="6"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="5"/>
-    <tableColumn id="10" name="date" dataDxfId="4"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="3">
+    <tableColumn id="1" name="title" dataDxfId="34"/>
+    <tableColumn id="2" name="authors" dataDxfId="33"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="32"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="31"/>
+    <tableColumn id="10" name="date" dataDxfId="30"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="29">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4571,10 +4636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U224"/>
+  <dimension ref="A1:U226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A222" sqref="A222"/>
+    <sheetView topLeftCell="A188" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A226" sqref="A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16124,7 +16189,7 @@
         <v>1005</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="C212" s="7" t="s">
         <v>509</v>
@@ -16142,7 +16207,7 @@
         <v>14</v>
       </c>
       <c r="H212" s="18" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="I212" s="18" t="s">
         <v>14</v>
@@ -16158,7 +16223,7 @@
       </c>
       <c r="M212" s="11"/>
       <c r="N212" s="19" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="O212" s="7"/>
       <c r="P212" s="24"/>
@@ -16195,7 +16260,7 @@
         <v>101</v>
       </c>
       <c r="H213" s="18" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="I213" s="18" t="s">
         <v>14</v>
@@ -16211,7 +16276,7 @@
       </c>
       <c r="M213" s="11"/>
       <c r="N213" s="19" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="O213" s="7"/>
       <c r="P213" s="24"/>
@@ -16227,16 +16292,16 @@
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="B214" s="7" t="s">
         <v>926</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="E214" s="18">
         <v>2023</v>
@@ -16264,7 +16329,7 @@
       </c>
       <c r="M214" s="11"/>
       <c r="N214" s="19" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="O214" s="7"/>
       <c r="P214" s="24"/>
@@ -16280,7 +16345,7 @@
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="B215" s="7" t="s">
         <v>971</v>
@@ -16370,7 +16435,7 @@
       </c>
       <c r="M216" s="11"/>
       <c r="N216" s="19" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="O216" s="7"/>
       <c r="P216" s="24"/>
@@ -16439,7 +16504,7 @@
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>1090</v>
+        <v>1085</v>
       </c>
       <c r="B218" s="7" t="s">
         <v>982</v>
@@ -16476,7 +16541,7 @@
       </c>
       <c r="M218" s="11"/>
       <c r="N218" s="19" t="s">
-        <v>1091</v>
+        <v>1086</v>
       </c>
       <c r="O218" s="7"/>
       <c r="P218" s="24"/>
@@ -16492,7 +16557,7 @@
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="B219" s="7" t="s">
         <v>767</v>
@@ -16529,7 +16594,7 @@
       </c>
       <c r="M219" s="11"/>
       <c r="N219" s="19" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="O219" s="7"/>
       <c r="P219" s="24"/>
@@ -16582,7 +16647,7 @@
       </c>
       <c r="M220" s="11"/>
       <c r="N220" s="19" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="O220" s="7"/>
       <c r="P220" s="24"/>
@@ -16619,7 +16684,7 @@
         <v>92</v>
       </c>
       <c r="H221" s="18" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="I221" s="18" t="s">
         <v>14</v>
@@ -16635,7 +16700,7 @@
       </c>
       <c r="M221" s="11"/>
       <c r="N221" s="19" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
       <c r="O221" s="7"/>
       <c r="P221" s="24"/>
@@ -16654,7 +16719,7 @@
         <v>1015</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>1088</v>
+        <v>1083</v>
       </c>
       <c r="C222" s="7" t="s">
         <v>1016</v>
@@ -16688,7 +16753,7 @@
       </c>
       <c r="M222" s="11"/>
       <c r="N222" s="19" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="O222" s="7"/>
       <c r="P222" s="24"/>
@@ -16753,7 +16818,7 @@
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="13" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="B224" s="13" t="s">
         <v>1014</v>
@@ -16783,14 +16848,14 @@
         <v>14</v>
       </c>
       <c r="K224" s="31">
-        <v>45295</v>
+        <v>45293</v>
       </c>
       <c r="L224" s="31" t="s">
         <v>273</v>
       </c>
       <c r="M224" s="45"/>
       <c r="N224" s="44" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
       <c r="O224" s="27"/>
       <c r="P224" s="24"/>
@@ -16800,100 +16865,202 @@
       <c r="T224" s="7"/>
       <c r="U224" s="7"/>
     </row>
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A225" s="13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B225" s="13" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C225" s="13" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D225" s="13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E225" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F225" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G225" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H225" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I225" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J225" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K225" s="31">
+        <v>45295</v>
+      </c>
+      <c r="L225" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="M225" s="45"/>
+      <c r="N225" s="44"/>
+      <c r="O225" s="27"/>
+      <c r="P225" s="24"/>
+      <c r="Q225" s="25"/>
+      <c r="R225" s="7"/>
+      <c r="S225" s="7"/>
+      <c r="T225" s="7"/>
+      <c r="U225" s="7"/>
+    </row>
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A226" s="13" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B226" s="13" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C226" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D226" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="E226" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F226" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G226" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H226" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I226" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J226" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K226" s="31">
+        <v>45294</v>
+      </c>
+      <c r="L226" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="M226" s="45"/>
+      <c r="N226" s="44"/>
+      <c r="O226" s="27"/>
+      <c r="P226" s="24"/>
+      <c r="Q226" s="25"/>
+      <c r="R226" s="7"/>
+      <c r="S226" s="7"/>
+      <c r="T226" s="7"/>
+      <c r="U226" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S148:U175 S136:U146 S177:U179 S182:U188 S190:U205 S207:U1048576">
-    <cfRule type="cellIs" dxfId="77" priority="25" operator="equal">
+  <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S148:U175 S136:U146 S177:U179 S182:U188 S190:U205 S207:U225 S227:U1048576">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="75" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="73" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="71" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="67" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S147:U147">
-    <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S176:U176">
-    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S181:U181">
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S189:U189">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S206:U206">
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S180:U180">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S226:U226">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16907,9 +17074,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17238,8 +17407,8 @@
       <c r="D11" s="7" t="s">
         <v>949</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>14</v>
+      <c r="E11" s="18">
+        <v>2023</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>14</v>
@@ -17253,6 +17422,36 @@
       <c r="I11" s="11"/>
       <c r="J11" s="19" t="s">
         <v>948</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>950</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>949</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2023</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="42">
+        <v>44927</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="19" t="s">
+        <v>1155</v>
       </c>
     </row>
   </sheetData>
@@ -17265,10 +17464,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17321,8 +17520,8 @@
         <v>44734</v>
       </c>
       <c r="G2" s="12">
-        <f t="shared" ref="G2:G16" ca="1" si="0">TODAY()-F2</f>
-        <v>340</v>
+        <f ca="1">TODAY()-F2</f>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -17339,14 +17538,14 @@
         <v>262</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="F3" s="10">
         <v>44769</v>
       </c>
       <c r="G3" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>305</v>
+        <f ca="1">TODAY()-F3</f>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -17367,8 +17566,8 @@
         <v>44803</v>
       </c>
       <c r="G4" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>271</v>
+        <f ca="1">TODAY()-F4</f>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -17389,8 +17588,8 @@
         <v>44832</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>242</v>
+        <f ca="1">TODAY()-F5</f>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -17411,8 +17610,8 @@
         <v>44883</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>191</v>
+        <f ca="1">TODAY()-F6</f>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -17433,16 +17632,16 @@
         <v>44904</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <f ca="1">TODAY()-F7</f>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1089</v>
+        <v>1033</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>1030</v>
@@ -17455,253 +17654,253 @@
         <v>44914</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <f ca="1">TODAY()-F8</f>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>1032</v>
+        <v>1056</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1033</v>
+        <v>1057</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1030</v>
+        <v>259</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1031</v>
+        <v>262</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="10">
-        <v>44914</v>
+        <v>44942</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <f ca="1">TODAY()-F9</f>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>1059</v>
+        <v>1067</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1060</v>
+        <v>1068</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>262</v>
+        <v>28</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="10">
-        <v>44942</v>
+        <v>44958</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>132</v>
+        <f ca="1">TODAY()-F10</f>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>1071</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>1072</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="10">
-        <v>44958</v>
+        <v>44959</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>116</v>
+        <f ca="1">TODAY()-F11</f>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>1074</v>
+        <v>1087</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1075</v>
+        <v>1090</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>120</v>
+        <v>1088</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>121</v>
+        <v>1089</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="10">
-        <v>44959</v>
+        <v>45013</v>
       </c>
       <c r="G12" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>115</v>
+        <f ca="1">TODAY()-F12</f>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>1084</v>
+        <v>1091</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1087</v>
+        <v>1094</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1086</v>
+        <v>1092</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>1085</v>
+        <v>1093</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="10">
-        <v>45008</v>
+        <v>45018</v>
       </c>
       <c r="G13" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <f ca="1">TODAY()-F13</f>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>1094</v>
+        <v>344</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="10">
-        <v>45013</v>
+        <v>45021</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <f ca="1">TODAY()-F14</f>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>1099</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>1097</v>
-      </c>
       <c r="D15" s="7" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="10">
-        <v>45018</v>
+        <v>45021</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <f ca="1">TODAY()-F15</f>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>344</v>
+        <v>1105</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="10">
-        <v>45021</v>
+        <v>45023</v>
       </c>
       <c r="G16" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <f ca="1">TODAY()-F16</f>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>1103</v>
+        <v>1110</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1106</v>
+        <v>1111</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>1104</v>
+        <v>1112</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>1105</v>
+        <v>1113</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="10">
-        <v>45021</v>
+        <v>45037</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" ref="G17:G20" ca="1" si="1">TODAY()-F17</f>
-        <v>53</v>
+        <f ca="1">TODAY()-F17</f>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>1108</v>
+        <v>1115</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>1109</v>
+        <v>1099</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>1110</v>
+        <v>1100</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="10">
-        <v>45023</v>
+        <v>45043</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">TODAY()-F18</f>
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1117</v>
+        <v>89</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>1118</v>
+        <v>89</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="10">
-        <v>45037</v>
+        <v>45043</v>
       </c>
       <c r="G19" s="12">
-        <f t="shared" ca="1" si="1"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F19</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>1119</v>
       </c>
@@ -17709,108 +17908,86 @@
         <v>1120</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>1104</v>
+        <v>1128</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>1105</v>
+        <v>1127</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="10">
-        <v>45043</v>
+        <v>45061</v>
       </c>
       <c r="G20" s="12">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F20</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>1121</v>
+        <v>1129</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>1122</v>
+        <v>1132</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>89</v>
+        <v>1130</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>89</v>
+        <v>1131</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="10">
-        <v>45043</v>
+        <v>45063</v>
       </c>
       <c r="G21" s="12">
-        <f t="shared" ref="G21" ca="1" si="2">TODAY()-F21</f>
+        <f ca="1">TODAY()-F21</f>
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>1124</v>
+        <v>1139</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>1125</v>
+        <v>1140</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>1133</v>
+        <v>267</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>268</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>1141</v>
+      </c>
       <c r="F22" s="10">
-        <v>45061</v>
+        <v>45064</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" ref="G22" ca="1" si="3">TODAY()-F22</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F22</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>1134</v>
+        <v>1102</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>1137</v>
+        <v>1158</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>1135</v>
+        <v>1159</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>1136</v>
+        <v>1160</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="10">
-        <v>45063</v>
+        <v>45072</v>
       </c>
       <c r="G23" s="12">
-        <f t="shared" ref="G23:G24" ca="1" si="4">TODAY()-F23</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>1146</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>1144</v>
-      </c>
-      <c r="F24" s="10">
-        <v>45064</v>
-      </c>
-      <c r="G24" s="12">
-        <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <f ca="1">TODAY()-F23</f>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -17824,7 +18001,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
@@ -17837,7 +18014,7 @@
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -17857,7 +18034,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>168</v>
       </c>
@@ -17875,10 +18052,10 @@
       </c>
       <c r="F2" s="40">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>7.5780821917808217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7.6328767123287671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>169</v>
       </c>
@@ -17896,10 +18073,10 @@
       </c>
       <c r="F3" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5780821917808217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7.6328767123287671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>256</v>
       </c>
@@ -17917,10 +18094,10 @@
       </c>
       <c r="F4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>6.956164383561644</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7.0109589041095894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>346</v>
       </c>
@@ -17938,8 +18115,27 @@
       </c>
       <c r="F5" s="40">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>5.3260273972602743</v>
-      </c>
+        <v>5.3808219178082188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10">
+        <v>45077</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17951,11 +18147,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17980,197 +18174,231 @@
       </c>
       <c r="H1" s="50">
         <f>COUNTA(H3:H998)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" s="50">
         <f>COUNTA(I3:I998)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" s="51">
         <f>SUM(E1:I1)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B2" s="52" t="s">
         <v>175</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="E2" s="53" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G2" s="53" t="s">
         <v>1039</v>
       </c>
-      <c r="F2" s="53" t="s">
-        <v>1038</v>
-      </c>
-      <c r="G2" s="53" t="s">
+      <c r="H2" s="53" t="s">
         <v>1040</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="I2" s="53" t="s">
         <v>1041</v>
-      </c>
-      <c r="I2" s="53" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1037</v>
+        <v>1147</v>
       </c>
       <c r="B3" s="49" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C3" s="49" t="s">
         <v>1044</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>1045</v>
-      </c>
       <c r="D3" s="15" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C4" s="49" t="s">
         <v>1046</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>1047</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>1048</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="I4" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1049</v>
+        <v>1145</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1061</v>
+        <v>1144</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1078</v>
+        <v>1143</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>1079</v>
+        <v>1074</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="H7" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>1082</v>
+        <v>1077</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>1083</v>
+        <v>1078</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1140</v>
+        <v>1135</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>1141</v>
+        <v>1136</v>
       </c>
       <c r="C11" s="49" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>1142</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>1052</v>
-      </c>
-      <c r="I11" s="48" t="s">
-        <v>1043</v>
+      <c r="B12" s="49" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
@@ -18206,8 +18434,12 @@
     <hyperlink ref="C10" r:id="rId16"/>
     <hyperlink ref="B11" r:id="rId17"/>
     <hyperlink ref="C11" r:id="rId18"/>
+    <hyperlink ref="B12" r:id="rId19"/>
+    <hyperlink ref="C12" r:id="rId20"/>
+    <hyperlink ref="B13" r:id="rId21"/>
+    <hyperlink ref="C13" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new submitted and accepted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,9 @@
     <sheet name="zzz" sheetId="5" r:id="rId4"/>
     <sheet name="SCI" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">SCI!$A$2:$I$33</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="1233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="1274">
   <si>
     <t>title</t>
   </si>
@@ -3216,9 +3219,6 @@
     <t>Cruz Oliveira, Claudia; Charalampous, Periklis; Delaye, Julien; Grad, Diana Alecsandra; Kolkhir, Pavel; Mechili, Enkeleint A.; Unim, Brigid; Devleesschauwer, Brecht; Haagsma, Juanita A.</t>
   </si>
   <si>
-    <t>10.1101/2023.01.31.23285233</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bacterial antimicrobial resistance: Data gaps and relationships between human and animal resistance </t>
   </si>
   <si>
@@ -3294,9 +3294,6 @@
     <t>BMC Infectious Disease</t>
   </si>
   <si>
-    <t>Etiological and prognostic roles of frailty and multimorbidity in the development of SARS-CoV-2 health outcomes: systematic review of population-based studies</t>
-  </si>
-  <si>
     <t>Age and Ageing</t>
   </si>
   <si>
@@ -3333,12 +3330,6 @@
     <t>J. Public Health</t>
   </si>
   <si>
-    <t>Validation of the Global Burden of Disease study frailty index (GBD-FI) in the Survey of Health, Ageing and Retirement in Europe</t>
-  </si>
-  <si>
-    <t>O'Caoimh, Rónán; O'Donovan, Mark; Devleesschauwer, Brecht; Sezgin, Duygu; Aaron, Liew; Kabir, Zubair</t>
-  </si>
-  <si>
     <t>The direct disease burden of COVID-19 in Belgium in 2020 and 2021</t>
   </si>
   <si>
@@ -3486,9 +3477,6 @@
     <t>https://pubmed.ncbi.nlm.nih.gov/37184579/</t>
   </si>
   <si>
-    <t>Product promotional strategies in supermarkets and their effects on sales: A case study of breakfast cereals and drinks in New Zealand</t>
-  </si>
-  <si>
     <t>The Africa Food Environment Research Network (FERN): from concept to practice</t>
   </si>
   <si>
@@ -3555,9 +3543,6 @@
     <t>https://pubmed.ncbi.nlm.nih.gov/37480028/</t>
   </si>
   <si>
-    <t>Malaria drug resistance landscape in the Democratic Republic of the Congo: a spatial mapping systematic review of molecular surveillance surveys</t>
-  </si>
-  <si>
     <t>Kalenda Kayiba, Nadine; Tshibangu-Kabamba, Evariste; Rosas-Aguirre, Angel; Kaku, Natsuko; Nakagama, Yu; Kaneko, Akira; Makaba Mvumbi, Dieudonné; Malekita Yobi, Doudou; Devleesschauwer, Brecht; Losimba Likwela, Joris; Kabututu Zakayi, Pius; DeMol, Patrick; Lelo Mvumbi, Georges; Hayette, Marie-Pierre; Dikassa Lusamba, Paul; Kido, Yasutoshi; Speybroeck, Niko</t>
   </si>
   <si>
@@ -3724,6 +3709,147 @@
   </si>
   <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/37815372/</t>
+  </si>
+  <si>
+    <t>The landscape of drug resistance in Plasmodium falciparum malaria in the Democratic Republic of Congo: a mapping systematic review</t>
+  </si>
+  <si>
+    <t>Tropical Medicine and Health</t>
+  </si>
+  <si>
+    <t>Trop. Med. Health</t>
+  </si>
+  <si>
+    <t>10.1186/s41182-023-00551-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linking health survey data with health insurance data: methodology, challenges, opportunities and recommendations for public health research. An experience from the HISlink project in Belgium </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13690-023-01213-0</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37968754/</t>
+  </si>
+  <si>
+    <t>Attributing Ethiopian animal health losses to high-level causes using expert elicitation</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.prevetmed.2023.106077</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37976968/</t>
+  </si>
+  <si>
+    <t>Association between adherence to the EAT-Lancet sustainable reference diet and cardiovascular health among European adolescents: the HELENA study</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41430-023-01379-4</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/38093098/</t>
+  </si>
+  <si>
+    <t>Evaluation of an electrochemical sensor and comparison with spectroscopic approaches as used today in practice for harm reduction in a festival setting-A case study: Analysis of 3,4-methylenedioxymethamphetamine samples</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/38086368/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/dta.3625</t>
+  </si>
+  <si>
+    <t>Age-Specific Quantification of Overweight/Obesity Risk Factors From Infancy to Adolescence and Differences by Educational Level of Parents</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/ijph.2023.1605798</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/38033763/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparing frailty prevalence between countries: validation of the Global Burden of Disease study Frailty Index (GBD-FI) in the survey of health, ageing and retirement in Europe </t>
+  </si>
+  <si>
+    <t>O'Donovan, Mark R; Devleesschauwer, Brecht; Sezgin, Duygu; Liew, Aaron; Kabir, Zubair; O'Caoimh, Rónán</t>
+  </si>
+  <si>
+    <t>afad214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1093/ageing/afad214 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient Reported Outcome and Experience Measures (PROMs and PREMs) in substance use disorder treatment services: A scoping review </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.drugalcdep.2023.111017</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37995391/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependence-Robust Confidence Intervals for Capture-Recapture Surveys </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/jssam/smac031</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37975066/</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>overview of available/added</t>
+  </si>
+  <si>
+    <t>check link to projects, health topics, authors</t>
+  </si>
+  <si>
+    <t>add PDF</t>
+  </si>
+  <si>
+    <t>Email Stefanie</t>
+  </si>
+  <si>
+    <t>list to add</t>
+  </si>
+  <si>
+    <t>Uncovering the toll of the first three COVID-19 waves: excess mortality and social patterns in Belgium</t>
+  </si>
+  <si>
+    <t>Van den Borre, Laura; Gadeyne, Sylvie; Devleesschauwer, Brecht; Vanthomme, Katrien</t>
+  </si>
+  <si>
+    <t>SSM - Population Health</t>
+  </si>
+  <si>
+    <t>SSM - Popul. Health</t>
+  </si>
+  <si>
+    <t>Santos, João Vasco; Padron Monedero, Alicia; Bikbov, Boris; Grad, Diana Alecsandra; Plass, Dietrich; Mechili, Enkeleint A; Gazzelloni, Federica; Fischer, Florian; Sulo, Gerhard; Ngwa, Che Henry; Noguer-Zambrano, Isabel; Peñalvo, José Luis; Haagsma, Juanita A; Kissmiova-Skarbek, Katarzyna; Monasta, Lorenzo; Ghith, Nermin; Sarmiento-Suarez, Rodrigo; Hrzic, Rok; Haneef, Romana; O'Caoimh, Rónán; Cuschieri, Sarah; Mondello, Stefania; Kabir, Zubair; Freitas, Alberto; Devleesschauwer, Brecht; GBD 2019 EU State of Health Collaborators</t>
+  </si>
+  <si>
+    <t>Multimorbidity and frailty are associated with poorer SARS-CoV-2-related outcomes: systematic review of population-based studies</t>
+  </si>
+  <si>
+    <t>Aging Clinical and Experimental Research</t>
+  </si>
+  <si>
+    <t>Aging Clin. Exp. Res.</t>
+  </si>
+  <si>
+    <t>Journal of Transport and Health</t>
+  </si>
+  <si>
+    <t>Vandeninden, Bram; De Clercq, Eva; Devleesschauwer, Brecht; Otavova, Martina; Masquelier, Bruno; Fierens, Frans; Faes, Christel; Bouland, Catherine</t>
+  </si>
+  <si>
+    <t>Methodology for assessing the impact of local traffic interventions on disease burden: a case study on paediatric asthma incidence in European cities</t>
   </si>
 </sst>
 </file>
@@ -4013,7 +4139,137 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4218,66 +4474,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -4292,74 +4488,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U244" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:U244"/>
-  <sortState ref="A2:U244">
-    <sortCondition ref="K1:K244"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U247" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+  <autoFilter ref="A1:U247"/>
+  <sortState ref="A2:U246">
+    <sortCondition ref="K1:K246"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="52"/>
-    <tableColumn id="2" name="authors" dataDxfId="51"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="50"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="49"/>
-    <tableColumn id="6" name="year" dataDxfId="48"/>
-    <tableColumn id="4" name="volume" dataDxfId="47"/>
-    <tableColumn id="5" name="issue" dataDxfId="46"/>
-    <tableColumn id="7" name="eID" dataDxfId="45"/>
-    <tableColumn id="8" name="from" dataDxfId="44"/>
-    <tableColumn id="9" name="to" dataDxfId="43"/>
-    <tableColumn id="10" name="date" dataDxfId="42"/>
-    <tableColumn id="19" name="date_submitted" dataDxfId="41" dataCellStyle="Neutral"/>
-    <tableColumn id="14" name="classification" dataDxfId="40"/>
-    <tableColumn id="12" name="IF" dataDxfId="39"/>
-    <tableColumn id="13" name="DOI" dataDxfId="38"/>
-    <tableColumn id="15" name="WoS" dataDxfId="37"/>
-    <tableColumn id="16" name="rank" dataDxfId="36"/>
-    <tableColumn id="17" name="quartile" dataDxfId="35"/>
-    <tableColumn id="18" name="category" dataDxfId="34"/>
-    <tableColumn id="20" name="SC" dataDxfId="33"/>
-    <tableColumn id="21" name="UGent" dataDxfId="32"/>
+    <tableColumn id="1" name="title" dataDxfId="65"/>
+    <tableColumn id="2" name="authors" dataDxfId="64"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="63"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="62"/>
+    <tableColumn id="6" name="year" dataDxfId="61"/>
+    <tableColumn id="4" name="volume" dataDxfId="60"/>
+    <tableColumn id="5" name="issue" dataDxfId="59"/>
+    <tableColumn id="7" name="eID" dataDxfId="58"/>
+    <tableColumn id="8" name="from" dataDxfId="57"/>
+    <tableColumn id="9" name="to" dataDxfId="56"/>
+    <tableColumn id="10" name="date" dataDxfId="55"/>
+    <tableColumn id="19" name="date_submitted" dataDxfId="54" dataCellStyle="Neutral"/>
+    <tableColumn id="14" name="classification" dataDxfId="53"/>
+    <tableColumn id="12" name="IF" dataDxfId="52"/>
+    <tableColumn id="13" name="DOI" dataDxfId="51"/>
+    <tableColumn id="15" name="WoS" dataDxfId="50"/>
+    <tableColumn id="16" name="rank" dataDxfId="49"/>
+    <tableColumn id="17" name="quartile" dataDxfId="48"/>
+    <tableColumn id="18" name="category" dataDxfId="47"/>
+    <tableColumn id="20" name="SC" dataDxfId="46"/>
+    <tableColumn id="21" name="UGent" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J12" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J12" totalsRowShown="0" headerRowDxfId="44">
   <autoFilter ref="A1:J12"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="30"/>
-    <tableColumn id="2" name="authors" dataDxfId="29"/>
-    <tableColumn id="3" name="editors" dataDxfId="28"/>
-    <tableColumn id="11" name="book" dataDxfId="27"/>
-    <tableColumn id="6" name="year" dataDxfId="26"/>
-    <tableColumn id="8" name="from" dataDxfId="25"/>
-    <tableColumn id="9" name="to" dataDxfId="24"/>
-    <tableColumn id="10" name="date" dataDxfId="23"/>
-    <tableColumn id="12" name="IF" dataDxfId="22"/>
-    <tableColumn id="13" name="DOI" dataDxfId="21"/>
+    <tableColumn id="1" name="title" dataDxfId="43"/>
+    <tableColumn id="2" name="authors" dataDxfId="42"/>
+    <tableColumn id="3" name="editors" dataDxfId="41"/>
+    <tableColumn id="11" name="book" dataDxfId="40"/>
+    <tableColumn id="6" name="year" dataDxfId="39"/>
+    <tableColumn id="8" name="from" dataDxfId="38"/>
+    <tableColumn id="9" name="to" dataDxfId="37"/>
+    <tableColumn id="10" name="date" dataDxfId="36"/>
+    <tableColumn id="12" name="IF" dataDxfId="35"/>
+    <tableColumn id="13" name="DOI" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:G13" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:G13" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:G13"/>
-  <sortState ref="A2:G15">
-    <sortCondition ref="F1:F15"/>
+  <sortState ref="A2:G13">
+    <sortCondition ref="F1:F13"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="title" dataDxfId="18"/>
-    <tableColumn id="2" name="authors" dataDxfId="17"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="16"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="15"/>
-    <tableColumn id="4" name="doi_preprint" dataDxfId="14"/>
-    <tableColumn id="10" name="date" dataDxfId="13"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="12">
+    <tableColumn id="1" name="title" dataDxfId="31"/>
+    <tableColumn id="2" name="authors" dataDxfId="30"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="29"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="28"/>
+    <tableColumn id="4" name="doi_preprint" dataDxfId="27"/>
+    <tableColumn id="10" name="date" dataDxfId="26"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="25">
       <calculatedColumnFormula>TODAY()-F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4368,18 +4564,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="9"/>
-    <tableColumn id="2" name="authors" dataDxfId="8"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="7"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="6"/>
-    <tableColumn id="10" name="date" dataDxfId="5"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="4">
+    <tableColumn id="1" name="title" dataDxfId="22"/>
+    <tableColumn id="2" name="authors" dataDxfId="21"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="20"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="19"/>
+    <tableColumn id="10" name="date" dataDxfId="18"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="17">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4674,10 +4870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U244"/>
+  <dimension ref="A1:U247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A241" sqref="A241"/>
+    <sheetView topLeftCell="A209" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A247" sqref="A247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4732,7 +4928,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>272</v>
@@ -16245,7 +16441,7 @@
         <v>14</v>
       </c>
       <c r="H212" s="18" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="I212" s="18" t="s">
         <v>14</v>
@@ -16383,7 +16579,7 @@
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B215" s="7" t="s">
         <v>970</v>
@@ -16542,7 +16738,7 @@
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B218" s="7" t="s">
         <v>981</v>
@@ -16580,7 +16776,7 @@
       </c>
       <c r="N218" s="11"/>
       <c r="O218" s="19" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="P218" s="7"/>
       <c r="Q218" s="24"/>
@@ -16595,7 +16791,7 @@
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B219" s="7" t="s">
         <v>766</v>
@@ -16633,7 +16829,7 @@
       </c>
       <c r="N219" s="11"/>
       <c r="O219" s="19" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="P219" s="7"/>
       <c r="Q219" s="24"/>
@@ -16686,7 +16882,7 @@
       </c>
       <c r="N220" s="11"/>
       <c r="O220" s="19" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="P220" s="7"/>
       <c r="Q220" s="24"/>
@@ -16722,7 +16918,7 @@
         <v>92</v>
       </c>
       <c r="H221" s="18" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="I221" s="18" t="s">
         <v>14</v>
@@ -16739,7 +16935,7 @@
       </c>
       <c r="N221" s="11"/>
       <c r="O221" s="19" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="P221" s="7"/>
       <c r="Q221" s="24"/>
@@ -16754,7 +16950,7 @@
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="B222" s="7" t="s">
         <v>1013</v>
@@ -16792,7 +16988,7 @@
       </c>
       <c r="N222" s="11"/>
       <c r="O222" s="19" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="P222" s="7"/>
       <c r="Q222" s="24"/>
@@ -16810,7 +17006,7 @@
         <v>1014</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C223" s="7" t="s">
         <v>1015</v>
@@ -16845,7 +17041,7 @@
       </c>
       <c r="N223" s="11"/>
       <c r="O223" s="19" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="P223" s="7"/>
       <c r="Q223" s="24"/>
@@ -16863,7 +17059,7 @@
         <v>1027</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C224" s="7" t="s">
         <v>267</v>
@@ -16898,7 +17094,7 @@
       </c>
       <c r="N224" s="11"/>
       <c r="O224" s="19" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="P224" s="7"/>
       <c r="Q224" s="24"/>
@@ -16951,7 +17147,7 @@
       </c>
       <c r="N225" s="11"/>
       <c r="O225" s="19" t="s">
-        <v>1178</v>
+        <v>1172</v>
       </c>
       <c r="P225" s="7"/>
       <c r="Q225" s="24"/>
@@ -16966,16 +17162,16 @@
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="D226" s="7" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="E226" s="18">
         <v>2023</v>
@@ -17004,7 +17200,7 @@
       </c>
       <c r="N226" s="11"/>
       <c r="O226" s="19" t="s">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="P226" s="7"/>
       <c r="Q226" s="24"/>
@@ -17019,10 +17215,10 @@
     </row>
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="C227" s="7" t="s">
         <v>509</v>
@@ -17040,7 +17236,7 @@
         <v>14</v>
       </c>
       <c r="H227" s="18" t="s">
-        <v>1205</v>
+        <v>1199</v>
       </c>
       <c r="I227" s="18" t="s">
         <v>14</v>
@@ -17057,7 +17253,7 @@
       </c>
       <c r="N227" s="11"/>
       <c r="O227" s="19" t="s">
-        <v>1193</v>
+        <v>1187</v>
       </c>
       <c r="P227" s="7"/>
       <c r="Q227" s="24"/>
@@ -17072,10 +17268,10 @@
     </row>
     <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>1198</v>
+        <v>1192</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>1199</v>
+        <v>1193</v>
       </c>
       <c r="C228" s="7" t="s">
         <v>267</v>
@@ -17110,7 +17306,7 @@
       </c>
       <c r="N228" s="11"/>
       <c r="O228" s="19" t="s">
-        <v>1200</v>
+        <v>1194</v>
       </c>
       <c r="P228" s="7"/>
       <c r="Q228" s="24"/>
@@ -17125,10 +17321,10 @@
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="C229" s="7" t="s">
         <v>267</v>
@@ -17163,7 +17359,7 @@
       </c>
       <c r="N229" s="11"/>
       <c r="O229" s="19" t="s">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="P229" s="7"/>
       <c r="Q229" s="24"/>
@@ -17178,10 +17374,10 @@
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="C230" s="7" t="s">
         <v>89</v>
@@ -17216,7 +17412,7 @@
       </c>
       <c r="N230" s="11"/>
       <c r="O230" s="19" t="s">
-        <v>1203</v>
+        <v>1197</v>
       </c>
       <c r="P230" s="7"/>
       <c r="Q230" s="24"/>
@@ -17231,10 +17427,10 @@
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
-        <v>1201</v>
+        <v>1195</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>1202</v>
+        <v>1196</v>
       </c>
       <c r="C231" s="7" t="s">
         <v>267</v>
@@ -17269,7 +17465,7 @@
       </c>
       <c r="N231" s="11"/>
       <c r="O231" s="19" t="s">
-        <v>1204</v>
+        <v>1198</v>
       </c>
       <c r="P231" s="7"/>
       <c r="Q231" s="24"/>
@@ -17284,16 +17480,16 @@
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B232" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C232" s="7" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D232" s="7" t="s">
         <v>1073</v>
-      </c>
-      <c r="B232" s="7" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C232" s="7" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D232" s="7" t="s">
-        <v>1074</v>
       </c>
       <c r="E232" s="18">
         <v>2023</v>
@@ -17322,7 +17518,7 @@
       </c>
       <c r="N232" s="11"/>
       <c r="O232" s="19" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="P232" s="7"/>
       <c r="Q232" s="24"/>
@@ -17375,7 +17571,7 @@
       </c>
       <c r="N233" s="11"/>
       <c r="O233" s="19" t="s">
-        <v>1189</v>
+        <v>1183</v>
       </c>
       <c r="P233" s="7"/>
       <c r="Q233" s="24"/>
@@ -17390,10 +17586,10 @@
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B234" s="7" t="s">
         <v>1085</v>
-      </c>
-      <c r="B234" s="7" t="s">
-        <v>1086</v>
       </c>
       <c r="C234" s="7" t="s">
         <v>144</v>
@@ -17411,7 +17607,7 @@
         <v>99</v>
       </c>
       <c r="H234" s="18" t="s">
-        <v>1209</v>
+        <v>1203</v>
       </c>
       <c r="I234" s="18" t="s">
         <v>14</v>
@@ -17428,7 +17624,7 @@
       </c>
       <c r="N234" s="11"/>
       <c r="O234" s="19" t="s">
-        <v>1211</v>
+        <v>1205</v>
       </c>
       <c r="P234" s="7"/>
       <c r="Q234" s="24"/>
@@ -17443,7 +17639,7 @@
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
-        <v>1212</v>
+        <v>1206</v>
       </c>
       <c r="B235" s="7" t="s">
         <v>1051</v>
@@ -17464,7 +17660,7 @@
         <v>99</v>
       </c>
       <c r="H235" s="18" t="s">
-        <v>1213</v>
+        <v>1207</v>
       </c>
       <c r="I235" s="18" t="s">
         <v>14</v>
@@ -17481,7 +17677,7 @@
       </c>
       <c r="N235" s="11"/>
       <c r="O235" s="19" t="s">
-        <v>1214</v>
+        <v>1208</v>
       </c>
       <c r="P235" s="7"/>
       <c r="Q235" s="24"/>
@@ -17517,7 +17713,7 @@
         <v>99</v>
       </c>
       <c r="H236" s="18" t="s">
-        <v>1219</v>
+        <v>1213</v>
       </c>
       <c r="I236" s="18" t="s">
         <v>14</v>
@@ -17534,7 +17730,7 @@
       </c>
       <c r="N236" s="11"/>
       <c r="O236" s="19" t="s">
-        <v>1220</v>
+        <v>1214</v>
       </c>
       <c r="P236" s="7"/>
       <c r="Q236" s="24"/>
@@ -17549,16 +17745,16 @@
     </row>
     <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="D237" s="7" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="E237" s="18">
         <v>2023</v>
@@ -17587,14 +17783,18 @@
       </c>
       <c r="N237" s="11"/>
       <c r="O237" s="19" t="s">
-        <v>1210</v>
+        <v>1204</v>
       </c>
       <c r="P237" s="7"/>
       <c r="Q237" s="24"/>
       <c r="R237" s="25"/>
       <c r="S237" s="7"/>
-      <c r="T237" s="7"/>
-      <c r="U237" s="7"/>
+      <c r="T237" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="U237" s="7" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
@@ -17636,13 +17836,15 @@
       </c>
       <c r="N238" s="11"/>
       <c r="O238" s="19" t="s">
-        <v>1221</v>
+        <v>1215</v>
       </c>
       <c r="P238" s="7"/>
       <c r="Q238" s="24"/>
       <c r="R238" s="25"/>
       <c r="S238" s="7"/>
-      <c r="T238" s="7"/>
+      <c r="T238" s="7" t="s">
+        <v>603</v>
+      </c>
       <c r="U238" s="7" t="s">
         <v>603</v>
       </c>
@@ -17655,10 +17857,10 @@
         <v>980</v>
       </c>
       <c r="C239" s="7" t="s">
-        <v>1224</v>
+        <v>1218</v>
       </c>
       <c r="D239" s="7" t="s">
-        <v>1225</v>
+        <v>1219</v>
       </c>
       <c r="E239" s="18">
         <v>2023</v>
@@ -17687,41 +17889,43 @@
       </c>
       <c r="N239" s="11"/>
       <c r="O239" s="19" t="s">
-        <v>1229</v>
+        <v>1223</v>
       </c>
       <c r="P239" s="7"/>
       <c r="Q239" s="24"/>
       <c r="R239" s="25"/>
       <c r="S239" s="7"/>
-      <c r="T239" s="7"/>
+      <c r="T239" s="7" t="s">
+        <v>603</v>
+      </c>
       <c r="U239" s="7" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
-        <v>1087</v>
+        <v>1246</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>1227</v>
+        <v>1247</v>
       </c>
       <c r="C240" s="7" t="s">
         <v>1088</v>
       </c>
       <c r="D240" s="7" t="s">
-        <v>344</v>
+        <v>1089</v>
       </c>
       <c r="E240" s="18">
         <v>2023</v>
       </c>
       <c r="F240" s="18">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G240" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H240" s="18">
-        <v>774</v>
+        <v>69</v>
+      </c>
+      <c r="H240" s="18" t="s">
+        <v>1248</v>
       </c>
       <c r="I240" s="18" t="s">
         <v>14</v>
@@ -17730,7 +17934,7 @@
         <v>14</v>
       </c>
       <c r="K240" s="42">
-        <v>45238</v>
+        <v>45232</v>
       </c>
       <c r="L240" s="42"/>
       <c r="M240" s="42" t="s">
@@ -17738,41 +17942,43 @@
       </c>
       <c r="N240" s="11"/>
       <c r="O240" s="19" t="s">
-        <v>1228</v>
+        <v>1249</v>
       </c>
       <c r="P240" s="7"/>
       <c r="Q240" s="24"/>
       <c r="R240" s="25"/>
       <c r="S240" s="7"/>
-      <c r="T240" s="7"/>
+      <c r="T240" s="7" t="s">
+        <v>603</v>
+      </c>
       <c r="U240" s="7" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="241" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>1018</v>
+        <v>1086</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>1017</v>
+        <v>1221</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>419</v>
+        <v>1087</v>
       </c>
       <c r="D241" s="7" t="s">
-        <v>419</v>
+        <v>344</v>
       </c>
       <c r="E241" s="18">
         <v>2023</v>
       </c>
       <c r="F241" s="18">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G241" s="19" t="s">
         <v>14</v>
       </c>
       <c r="H241" s="18">
-        <v>100595</v>
+        <v>774</v>
       </c>
       <c r="I241" s="18" t="s">
         <v>14</v>
@@ -17781,7 +17987,7 @@
         <v>14</v>
       </c>
       <c r="K241" s="42">
-        <v>45261</v>
+        <v>45238</v>
       </c>
       <c r="L241" s="42"/>
       <c r="M241" s="42" t="s">
@@ -17789,7 +17995,7 @@
       </c>
       <c r="N241" s="11"/>
       <c r="O241" s="19" t="s">
-        <v>1164</v>
+        <v>1222</v>
       </c>
       <c r="P241" s="7"/>
       <c r="Q241" s="24"/>
@@ -17803,170 +18009,335 @@
       </c>
     </row>
     <row r="242" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A242" s="13" t="s">
-        <v>984</v>
-      </c>
-      <c r="B242" s="13" t="s">
-        <v>985</v>
-      </c>
-      <c r="C242" s="13" t="s">
-        <v>986</v>
-      </c>
-      <c r="D242" s="13" t="s">
-        <v>987</v>
-      </c>
-      <c r="E242" s="14">
+      <c r="A242" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B242" s="7" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C242" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D242" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E242" s="18">
         <v>2023</v>
       </c>
-      <c r="F242" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G242" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H242" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I242" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J242" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K242" s="31">
-        <v>45292</v>
-      </c>
-      <c r="L242" s="31"/>
-      <c r="M242" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="N242" s="45"/>
-      <c r="O242" s="44" t="s">
-        <v>991</v>
-      </c>
-      <c r="P242" s="27"/>
+      <c r="F242" s="18">
+        <v>51</v>
+      </c>
+      <c r="G242" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H242" s="18">
+        <v>64</v>
+      </c>
+      <c r="I242" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J242" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K242" s="42">
+        <v>45245</v>
+      </c>
+      <c r="L242" s="42"/>
+      <c r="M242" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="N242" s="11"/>
+      <c r="O242" s="19" t="s">
+        <v>1230</v>
+      </c>
+      <c r="P242" s="7"/>
       <c r="Q242" s="24"/>
       <c r="R242" s="25"/>
       <c r="S242" s="7"/>
-      <c r="T242" s="7"/>
-      <c r="U242" s="7"/>
+      <c r="T242" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="U242" s="7" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A243" s="13" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B243" s="13" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C243" s="13" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D243" s="13" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E243" s="14">
+      <c r="A243" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B243" s="7" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C243" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D243" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E243" s="18">
         <v>2023</v>
       </c>
-      <c r="F243" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G243" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H243" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I243" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J243" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K243" s="31">
-        <v>45296</v>
-      </c>
-      <c r="L243" s="31"/>
-      <c r="M243" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="N243" s="45"/>
-      <c r="O243" s="44"/>
-      <c r="P243" s="27"/>
+      <c r="F243" s="18">
+        <v>17</v>
+      </c>
+      <c r="G243" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H243" s="18">
+        <v>100595</v>
+      </c>
+      <c r="I243" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J243" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K243" s="42">
+        <v>45261</v>
+      </c>
+      <c r="L243" s="42"/>
+      <c r="M243" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="N243" s="11"/>
+      <c r="O243" s="19" t="s">
+        <v>1159</v>
+      </c>
+      <c r="P243" s="7"/>
       <c r="Q243" s="24"/>
       <c r="R243" s="25"/>
       <c r="S243" s="7"/>
-      <c r="T243" s="7"/>
-      <c r="U243" s="7"/>
+      <c r="T243" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="U243" s="7" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="244" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A244" s="13" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B244" s="13" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C244" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D244" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E244" s="14">
+      <c r="A244" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="B244" s="7" t="s">
+        <v>985</v>
+      </c>
+      <c r="C244" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="D244" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="E244" s="18">
         <v>2023</v>
       </c>
-      <c r="F244" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G244" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H244" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I244" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J244" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K244" s="31">
-        <v>45297</v>
-      </c>
-      <c r="L244" s="31"/>
-      <c r="M244" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="N244" s="45"/>
-      <c r="O244" s="44"/>
-      <c r="P244" s="27"/>
+      <c r="F244" s="18">
+        <v>19</v>
+      </c>
+      <c r="G244" s="19" t="s">
+        <v>548</v>
+      </c>
+      <c r="H244" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I244" s="18">
+        <v>743</v>
+      </c>
+      <c r="J244" s="18">
+        <v>757</v>
+      </c>
+      <c r="K244" s="42">
+        <v>45261</v>
+      </c>
+      <c r="L244" s="42"/>
+      <c r="M244" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="N244" s="11"/>
+      <c r="O244" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="P244" s="7"/>
       <c r="Q244" s="24"/>
       <c r="R244" s="25"/>
       <c r="S244" s="7"/>
-      <c r="T244" s="7"/>
-      <c r="U244" s="7"/>
+      <c r="T244" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="U244" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A245" s="13" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B245" s="13" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C245" s="13" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D245" s="13" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E245" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F245" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G245" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H245" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I245" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J245" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K245" s="31">
+        <v>45658</v>
+      </c>
+      <c r="L245" s="31"/>
+      <c r="M245" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="N245" s="45"/>
+      <c r="O245" s="44"/>
+      <c r="P245" s="27"/>
+      <c r="Q245" s="24"/>
+      <c r="R245" s="25"/>
+      <c r="S245" s="7"/>
+      <c r="T245" s="7"/>
+      <c r="U245" s="7"/>
+    </row>
+    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A246" s="13" t="s">
+        <v>971</v>
+      </c>
+      <c r="B246" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="C246" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D246" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E246" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F246" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G246" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H246" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I246" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J246" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K246" s="31">
+        <v>45659</v>
+      </c>
+      <c r="L246" s="31"/>
+      <c r="M246" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="N246" s="45"/>
+      <c r="O246" s="44"/>
+      <c r="P246" s="27"/>
+      <c r="Q246" s="24"/>
+      <c r="R246" s="25"/>
+      <c r="S246" s="7"/>
+      <c r="T246" s="7"/>
+      <c r="U246" s="7"/>
+    </row>
+    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A247" s="13" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B247" s="13" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C247" s="13" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D247" s="13" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E247" s="14">
+        <v>2023</v>
+      </c>
+      <c r="F247" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G247" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H247" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I247" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J247" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="K247" s="31">
+        <v>45660</v>
+      </c>
+      <c r="L247" s="31"/>
+      <c r="M247" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="N247" s="45"/>
+      <c r="O247" s="44"/>
+      <c r="P247" s="27"/>
+      <c r="Q247" s="24"/>
+      <c r="R247" s="25"/>
+      <c r="S247" s="7"/>
+      <c r="T247" s="7"/>
+      <c r="U247" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="T1:U112 T114:U231 T232:V240 T242:V1048576 V241">
-    <cfRule type="cellIs" dxfId="60" priority="29" operator="equal">
+  <conditionalFormatting sqref="T1:U112 T114:U231 T248:V1048576 V246:V247 T232:V240 V241:V242 T241:T242 T243:V245">
+    <cfRule type="cellIs" dxfId="12" priority="31" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="32" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="58" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="29" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="30" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T241:U241">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+  <conditionalFormatting sqref="U241:U242">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T246:U247">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18332,10 +18703,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>949</v>
@@ -18357,7 +18728,7 @@
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="19" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
     </row>
   </sheetData>
@@ -18370,11 +18741,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18385,7 +18754,7 @@
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -18407,283 +18776,278 @@
       <c r="G1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="55">
+      <c r="I1" s="55" t="str">
+        <f ca="1">ROUND(J1/30,0)&amp;" md"</f>
+        <v>6 md</v>
+      </c>
+      <c r="J1" s="55">
         <f ca="1">AVERAGE(G:G)</f>
-        <v>195.5</v>
-      </c>
-      <c r="J1" s="54" t="s">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>179.83333333333334</v>
+      </c>
+      <c r="K1" s="54" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>971</v>
+        <v>1061</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>972</v>
+        <v>1062</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="10">
+        <v>44958</v>
+      </c>
+      <c r="G2" s="12">
+        <f ca="1">TODAY()-F2</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>1063</v>
       </c>
-      <c r="F2" s="10">
-        <v>44769</v>
-      </c>
-      <c r="G2" s="12">
-        <f t="shared" ref="G2:G13" ca="1" si="0">TODAY()-F2</f>
-        <v>476</v>
-      </c>
-      <c r="I2" s="55" t="str">
-        <f ca="1">ROUND(I1/30,0)&amp;" md"</f>
-        <v>7 md</v>
-      </c>
-      <c r="J2" s="54"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>1061</v>
-      </c>
       <c r="B3" s="7" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="10">
-        <v>44958</v>
+        <v>44959</v>
       </c>
       <c r="G3" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F3</f>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>1064</v>
+        <v>1080</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>1065</v>
+        <v>1083</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>1081</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>121</v>
+        <v>1082</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="10">
-        <v>44959</v>
+        <v>45013</v>
       </c>
       <c r="G4" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F4</f>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>1081</v>
+        <v>1096</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1084</v>
+        <v>1097</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1082</v>
+        <v>1098</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1083</v>
+        <v>1099</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="10">
-        <v>45013</v>
+        <v>45037</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F5</f>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>1089</v>
+        <v>1139</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1092</v>
+        <v>1267</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1090</v>
+        <v>89</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1091</v>
+        <v>89</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="10">
-        <v>45021</v>
+        <v>45077</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F6</f>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>1098</v>
+        <v>1162</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>1099</v>
+        <v>1163</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1100</v>
+        <v>575</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1101</v>
+        <v>576</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="10">
-        <v>45037</v>
+        <v>45114</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F7</f>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>1102</v>
+        <v>1211</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1103</v>
+        <v>1212</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1090</v>
+        <v>160</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1091</v>
+        <v>161</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="10">
-        <v>45043</v>
+        <v>45116</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F8</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>1167</v>
+        <v>1181</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1168</v>
+        <v>1182</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>575</v>
+        <v>668</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>576</v>
+        <v>669</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="10">
-        <v>45114</v>
+        <v>45127</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F9</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>1217</v>
+        <v>1273</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1218</v>
+        <v>1272</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>161</v>
-      </c>
+        <v>1271</v>
+      </c>
+      <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="10">
-        <v>45116</v>
+        <v>45146</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F10</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>1187</v>
+        <v>1209</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1188</v>
+        <v>1220</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>668</v>
+        <v>259</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>669</v>
+        <v>262</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="10">
-        <v>45127</v>
+        <v>45208</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F11</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1226</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>259</v>
+        <v>160</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>262</v>
+        <v>161</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="10">
-        <v>45208</v>
+        <v>45229</v>
       </c>
       <c r="G12" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <f ca="1">TODAY()-F12</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>1222</v>
+        <v>1263</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1223</v>
+        <v>1264</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>160</v>
+        <v>1265</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>161</v>
+        <v>1266</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="10">
-        <v>45229</v>
+        <v>45278</v>
       </c>
       <c r="G13" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <f ca="1">TODAY()-F13</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -18748,7 +19112,7 @@
       </c>
       <c r="F2" s="40">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>8.0465753424657542</v>
+        <v>8.1561643835616433</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -18769,7 +19133,7 @@
       </c>
       <c r="F3" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0465753424657542</v>
+        <v>8.1561643835616433</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -18790,7 +19154,7 @@
       </c>
       <c r="F4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4246575342465757</v>
+        <v>7.5342465753424657</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -18811,21 +19175,21 @@
       </c>
       <c r="F5" s="40">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>5.7945205479452051</v>
+        <v>5.904109589041096</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>1143</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>1147</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="10">
@@ -18843,11 +19207,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18857,33 +19219,33 @@
     <col min="5" max="9" width="9.140625" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E1" s="50">
-        <f>COUNTA(E3:E998)</f>
-        <v>2</v>
+        <f>COUNTA(E3:E997)</f>
+        <v>3</v>
       </c>
       <c r="F1" s="50">
-        <f>COUNTA(F3:F998)</f>
-        <v>6</v>
+        <f>COUNTA(F3:F997)</f>
+        <v>7</v>
       </c>
       <c r="G1" s="50">
-        <f>COUNTA(G3:G998)</f>
-        <v>2</v>
+        <f>COUNTA(G3:G997)</f>
+        <v>5</v>
       </c>
       <c r="H1" s="50">
-        <f>COUNTA(H3:H998)</f>
-        <v>12</v>
+        <f>COUNTA(H3:H997)</f>
+        <v>13</v>
       </c>
       <c r="I1" s="50">
-        <f>COUNTA(I3:I998)</f>
+        <f>COUNTA(I3:I997)</f>
         <v>3</v>
       </c>
       <c r="J1" s="51">
         <f>SUM(E1:I1)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>1045</v>
       </c>
@@ -18897,7 +19259,7 @@
         <v>1047</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="F2" s="53" t="s">
         <v>1033</v>
@@ -18911,10 +19273,13 @@
       <c r="I2" s="53" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="53" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>1038</v>
@@ -18923,15 +19288,18 @@
         <v>1039</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1044</v>
+        <v>1256</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>1040</v>
@@ -18945,10 +19313,13 @@
       <c r="I4" s="48" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>1042</v>
@@ -18962,10 +19333,13 @@
       <c r="F5" s="48" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>1052</v>
@@ -18979,16 +19353,19 @@
       <c r="H6" s="48" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="B7" s="49" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C7" s="49" t="s">
         <v>1068</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>1069</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>1044</v>
@@ -18996,84 +19373,87 @@
       <c r="H7" s="48" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>1070</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="C8" s="49" t="s">
         <v>1071</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>1072</v>
-      </c>
       <c r="D8" s="15" t="s">
-        <v>1044</v>
+        <v>1055</v>
       </c>
       <c r="G8" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>1044</v>
+        <v>1256</v>
       </c>
       <c r="F9" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>1044</v>
+        <v>1256</v>
       </c>
       <c r="G10" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>1044</v>
+        <v>1256</v>
       </c>
       <c r="I11" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>1044</v>
@@ -19082,32 +19462,32 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>1044</v>
+        <v>1256</v>
       </c>
       <c r="I13" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>1044</v>
@@ -19116,49 +19496,46 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>1068</v>
+        <v>1150</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>1069</v>
+        <v>1151</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>1044</v>
+        <v>1055</v>
       </c>
       <c r="H15" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H16" s="48" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F16" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>1044</v>
+        <v>1055</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>1037</v>
@@ -19166,55 +19543,58 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>1160</v>
+        <v>1157</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>1158</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>1044</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="H18" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>1163</v>
+        <v>1166</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H19" s="48" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E19" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B20" s="49" t="s">
         <v>1169</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>1171</v>
+      <c r="C20" s="49" t="s">
+        <v>1170</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>1044</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="H20" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="C21" s="49" t="s">
         <v>1175</v>
@@ -19228,13 +19608,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C22" s="49" t="s">
         <v>1180</v>
-      </c>
-      <c r="B22" s="49" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>1181</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>1044</v>
@@ -19262,13 +19642,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B24" s="49" t="s">
         <v>1191</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>1044</v>
@@ -19279,72 +19659,180 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1195</v>
+        <v>1200</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>1197</v>
+        <v>1201</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>1196</v>
+        <v>1202</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H25" s="48" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F25" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1206</v>
+        <v>1224</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>1207</v>
+        <v>1225</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>1208</v>
+        <v>1226</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>1044</v>
-      </c>
-      <c r="F26" s="48" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E26" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D27" s="15" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>1044</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="H29" s="48" t="s">
         <v>1037</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>1256</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H31" s="48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G33" s="48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:I1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <autoFilter ref="A2:I33"/>
+  <conditionalFormatting sqref="E1:I1048576 L2">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1 D2:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"X"</formula>
+      <formula>"Added"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -19372,31 +19860,43 @@
     <hyperlink ref="C13" r:id="rId22"/>
     <hyperlink ref="B14" r:id="rId23"/>
     <hyperlink ref="C14" r:id="rId24"/>
-    <hyperlink ref="C15" r:id="rId25"/>
-    <hyperlink ref="B15" r:id="rId26"/>
+    <hyperlink ref="B15" r:id="rId25"/>
+    <hyperlink ref="C15" r:id="rId26"/>
     <hyperlink ref="B16" r:id="rId27"/>
-    <hyperlink ref="C16" r:id="rId28"/>
-    <hyperlink ref="B17" r:id="rId29"/>
-    <hyperlink ref="B18" r:id="rId30"/>
+    <hyperlink ref="B17" r:id="rId28"/>
+    <hyperlink ref="B18" r:id="rId29"/>
+    <hyperlink ref="C18" r:id="rId30"/>
     <hyperlink ref="B19" r:id="rId31"/>
-    <hyperlink ref="C19" r:id="rId32"/>
-    <hyperlink ref="B20" r:id="rId33"/>
-    <hyperlink ref="B21" r:id="rId34"/>
-    <hyperlink ref="C21" r:id="rId35"/>
-    <hyperlink ref="C22" r:id="rId36"/>
-    <hyperlink ref="B22" r:id="rId37"/>
+    <hyperlink ref="B20" r:id="rId32"/>
+    <hyperlink ref="C20" r:id="rId33"/>
+    <hyperlink ref="C21" r:id="rId34"/>
+    <hyperlink ref="B21" r:id="rId35"/>
+    <hyperlink ref="B22" r:id="rId36"/>
+    <hyperlink ref="C22" r:id="rId37"/>
     <hyperlink ref="B23" r:id="rId38"/>
     <hyperlink ref="C23" r:id="rId39"/>
-    <hyperlink ref="B24" r:id="rId40"/>
-    <hyperlink ref="C24" r:id="rId41"/>
-    <hyperlink ref="C25" r:id="rId42"/>
-    <hyperlink ref="B25" r:id="rId43"/>
-    <hyperlink ref="B26" r:id="rId44"/>
-    <hyperlink ref="C26" r:id="rId45"/>
-    <hyperlink ref="C27" r:id="rId46"/>
-    <hyperlink ref="B27" r:id="rId47"/>
+    <hyperlink ref="C24" r:id="rId40"/>
+    <hyperlink ref="B24" r:id="rId41"/>
+    <hyperlink ref="B25" r:id="rId42"/>
+    <hyperlink ref="C25" r:id="rId43"/>
+    <hyperlink ref="C26" r:id="rId44"/>
+    <hyperlink ref="B26" r:id="rId45"/>
+    <hyperlink ref="B27" r:id="rId46"/>
+    <hyperlink ref="C27" r:id="rId47"/>
+    <hyperlink ref="B28" r:id="rId48"/>
+    <hyperlink ref="C28" r:id="rId49"/>
+    <hyperlink ref="B29" r:id="rId50"/>
+    <hyperlink ref="C29" r:id="rId51"/>
+    <hyperlink ref="C30" r:id="rId52"/>
+    <hyperlink ref="B30" r:id="rId53"/>
+    <hyperlink ref="B31" r:id="rId54"/>
+    <hyperlink ref="C31" r:id="rId55"/>
+    <hyperlink ref="B32" r:id="rId56"/>
+    <hyperlink ref="C32" r:id="rId57"/>
+    <hyperlink ref="B33" r:id="rId58"/>
+    <hyperlink ref="C33" r:id="rId59"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>